<commit_message>
Test input with dollar feature
</commit_message>
<xml_diff>
--- a/migforecasting/less100/output.xlsx
+++ b/migforecasting/less100/output.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>227.6033649559943</v>
+        <v>479.3767310549769</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>348.2416184706817</v>
+        <v>473.5485038290082</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>319.4332357983764</v>
+        <v>469.2932929477648</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>358.8191450451475</v>
+        <v>633.3911647045371</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>330.9586055549199</v>
+        <v>434.9692696308142</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>770.9494273631263</v>
+        <v>224.4069150760089</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>741.4856212138518</v>
+        <v>590.8390558921017</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>4278.675041719051</v>
+        <v>4594.19590353183</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>3148.785468053491</v>
+        <v>4343.158628414675</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>3053.65831295005</v>
+        <v>5290.860642359125</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>2957.73456623614</v>
+        <v>5300.480242313406</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>594.4690936106978</v>
+        <v>906.8439227340259</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>3050.229943993597</v>
+        <v>4260.484519373642</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>637.9690456052117</v>
+        <v>871.0477174534225</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>1579.34874385644</v>
+        <v>1048.526311578465</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>885.1746142416267</v>
+        <v>1046.549957709452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>